<commit_message>
Casos de prueba ajustes 4
</commit_message>
<xml_diff>
--- a/Casos de Prueba.xlsx
+++ b/Casos de Prueba.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b12s307.B12_307_12.000\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932669EF-F65A-4E87-B1E5-A7251264A568}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A835793-247D-4EEF-AD90-2F15E03062A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -287,7 +287,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -510,12 +510,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -622,6 +659,21 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -907,7 +959,7 @@
   <dimension ref="A1:M16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="91" zoomScaleNormal="106" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,7 +997,7 @@
       <c r="L1" s="29"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="45" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -983,7 +1035,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="29"/>
+      <c r="A3" s="46"/>
       <c r="B3" s="5" t="s">
         <v>6</v>
       </c>
@@ -1019,7 +1071,9 @@
       </c>
     </row>
     <row r="4" spans="1:13" ht="69" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="29"/>
+      <c r="A4" s="47" t="s">
+        <v>4</v>
+      </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
@@ -1055,7 +1109,7 @@
       </c>
     </row>
     <row r="5" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
+      <c r="A5" s="48"/>
       <c r="B5" s="5" t="s">
         <v>24</v>
       </c>
@@ -1083,9 +1137,7 @@
       <c r="L5" s="31"/>
     </row>
     <row r="6" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
-        <v>4</v>
-      </c>
+      <c r="A6" s="48"/>
       <c r="B6" s="5" t="s">
         <v>23</v>
       </c>
@@ -1119,7 +1171,7 @@
       <c r="L6" s="31"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="48"/>
       <c r="B7" s="30" t="s">
         <v>44</v>
       </c>
@@ -1148,7 +1200,7 @@
       <c r="M7" s="2"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="31"/>
+      <c r="A8" s="49"/>
       <c r="B8" s="30"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -1272,8 +1324,8 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="A2:A5"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A8"/>
     <mergeCell ref="C1:E1"/>
     <mergeCell ref="F1:H1"/>
     <mergeCell ref="I1:L1"/>

</xml_diff>